<commit_message>
Fixed BOM and re-exported as xlsx file for pay-motors
</commit_message>
<xml_diff>
--- a/prototypes/pay-motors/Project Outputs for pay-motors-control/BOM/Bill of Materials-pay-motors-control.xlsx
+++ b/prototypes/pay-motors/Project Outputs for pay-motors-control/BOM/Bill of Materials-pay-motors-control.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9EAD2A4-0C1D-454C-9D24-865985D6F331}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E46AC883-3A61-41A7-AD07-5254F758F290}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2500" yWindow="1200" windowWidth="14400" windowHeight="9600" xr2:uid="{646257C5-5CC4-4237-BDB9-8384213137E4}"/>
+    <workbookView xWindow="2500" yWindow="1200" windowWidth="14400" windowHeight="9600" xr2:uid="{95593FA1-3CED-4E15-8656-EC22B7CFE0C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-pay-motors-co" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="174">
   <si>
     <t>Line #</t>
   </si>
@@ -100,10 +100,10 @@
     <t>Murata</t>
   </si>
   <si>
-    <t>GCM1555C1H150FA16D</t>
-  </si>
-  <si>
-    <t>490-14350-6-ND</t>
+    <t>GRM1555C1H150FA01D</t>
+  </si>
+  <si>
+    <t>490-6200-1-ND</t>
   </si>
   <si>
     <t>47uF</t>
@@ -124,7 +124,7 @@
     <t>New Product</t>
   </si>
   <si>
-    <t>565-4687-6-ND</t>
+    <t>565-4687-1-ND</t>
   </si>
   <si>
     <t>Cap 0603</t>
@@ -145,7 +145,7 @@
     <t>Volume Production</t>
   </si>
   <si>
-    <t>399-6856-6-ND</t>
+    <t>399-6856-1-ND</t>
   </si>
   <si>
     <t>Cap</t>
@@ -160,7 +160,7 @@
     <t>885012206001</t>
   </si>
   <si>
-    <t>732-7920-6-ND</t>
+    <t>732-7920-1-ND</t>
   </si>
   <si>
     <t>Cap 0805</t>
@@ -172,7 +172,7 @@
     <t>C0805F103K5RACAUTO</t>
   </si>
   <si>
-    <t>399-6982-6-ND</t>
+    <t>399-6982-1-ND</t>
   </si>
   <si>
     <t>LED2</t>
@@ -190,7 +190,7 @@
     <t>SML-D12U1WT86</t>
   </si>
   <si>
-    <t>SML-D12U1WT86DKR-ND</t>
+    <t>SML-D12U1WT86CT-ND</t>
   </si>
   <si>
     <t>GREEN LED</t>
@@ -205,7 +205,7 @@
     <t>SML-D12FWT86</t>
   </si>
   <si>
-    <t>846-1176-6-ND</t>
+    <t>846-1176-1-ND</t>
   </si>
   <si>
     <t>ORANGE LED</t>
@@ -217,7 +217,7 @@
     <t>SML-D12D8WT86</t>
   </si>
   <si>
-    <t>511-1577-6-ND</t>
+    <t>511-1577-1-ND</t>
   </si>
   <si>
     <t>D7, D8, D9</t>
@@ -328,13 +328,19 @@
     <t>Panasonic</t>
   </si>
   <si>
+    <t>ERJ-2RKF3002X</t>
+  </si>
+  <si>
+    <t>P30.0KLCT-ND</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
     <t>ERA-3AEB303V</t>
   </si>
   <si>
-    <t>P30KDBDKR-ND</t>
-  </si>
-  <si>
-    <t>R4</t>
+    <t>P30KDBCT-ND</t>
   </si>
   <si>
     <t>R5_DRV8843N1, R5_DRV8843N2, R8_DRV8843N1, R8_DRV8843N2</t>
@@ -355,7 +361,7 @@
     <t>MCT06030C1004FP500</t>
   </si>
   <si>
-    <t>MCT0603-1.00M-CFTR-ND</t>
+    <t>MCT0603-1.00M-CFCT-ND</t>
   </si>
   <si>
     <t>Res1</t>
@@ -391,6 +397,12 @@
     <t>R12, R13, R14, R15, R16, R17</t>
   </si>
   <si>
+    <t>ERJ3EKF3300V</t>
+  </si>
+  <si>
+    <t>P330HCT-ND</t>
+  </si>
+  <si>
     <t>10K</t>
   </si>
   <si>
@@ -448,7 +460,7 @@
     <t>PTS830GM140SMTRLFS</t>
   </si>
   <si>
-    <t>CKN10587DKR-ND</t>
+    <t>CKN10587CT-ND</t>
   </si>
   <si>
     <t>ATMega32M1</t>
@@ -929,7 +941,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{063AEA54-185C-419B-AC49-0D817C63ED01}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{289E77F6-7FCA-4D5B-8A0C-D79189FBE001}">
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1020,10 +1032,10 @@
         <v>20</v>
       </c>
       <c r="K2" s="3">
-        <v>0.13403000000000001</v>
+        <v>0.13411000000000001</v>
       </c>
       <c r="L2" s="3">
-        <v>0.67015000000000002</v>
+        <v>0.67054999999999998</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.4">
@@ -1058,10 +1070,10 @@
         <v>25</v>
       </c>
       <c r="K3" s="3">
-        <v>0.17424000000000001</v>
+        <v>0.13411000000000001</v>
       </c>
       <c r="L3" s="3">
-        <v>0.34848000000000001</v>
+        <v>0.26822000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.4">
@@ -1239,7 +1251,7 @@
         <v>53</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>19</v>
@@ -1286,10 +1298,10 @@
         <v>59</v>
       </c>
       <c r="K9" s="3">
-        <v>0.56291999999999998</v>
+        <v>0.56327000000000005</v>
       </c>
       <c r="L9" s="3">
-        <v>0.56291999999999998</v>
+        <v>0.56327000000000005</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.4">
@@ -1324,10 +1336,10 @@
         <v>63</v>
       </c>
       <c r="K10" s="3">
-        <v>0.45569999999999999</v>
+        <v>0.45598</v>
       </c>
       <c r="L10" s="3">
-        <v>0.91139999999999999</v>
+        <v>0.91195999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.4">
@@ -1624,10 +1636,10 @@
         <v>101</v>
       </c>
       <c r="K18" s="3">
-        <v>0.46910000000000002</v>
+        <v>0.13411000000000001</v>
       </c>
       <c r="L18" s="3">
-        <v>0.46910000000000002</v>
+        <v>0.13411000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="15" x14ac:dyDescent="0.4">
@@ -1650,7 +1662,7 @@
         <v>99</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>18</v>
@@ -1659,13 +1671,13 @@
         <v>19</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="K19" s="3">
-        <v>0.46910000000000002</v>
+        <v>0.46939999999999998</v>
       </c>
       <c r="L19" s="3">
-        <v>0.46910000000000002</v>
+        <v>0.46939999999999998</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="15" x14ac:dyDescent="0.4">
@@ -1679,7 +1691,7 @@
         <v>88</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E20" s="3">
         <v>4</v>
@@ -1688,7 +1700,7 @@
         <v>94</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>38</v>
@@ -1697,7 +1709,7 @@
         <v>19</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="K20" s="3">
         <v>0.26823000000000002</v>
@@ -1711,13 +1723,13 @@
         <v>12</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>88</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E21" s="3">
         <v>2</v>
@@ -1726,7 +1738,7 @@
         <v>90</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>38</v>
@@ -1735,13 +1747,13 @@
         <v>19</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="K21" s="3">
-        <v>2.5350000000000001E-2</v>
+        <v>0.2414</v>
       </c>
       <c r="L21" s="3">
-        <v>126.74</v>
+        <v>0.48281000000000002</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="15" x14ac:dyDescent="0.4">
@@ -1749,22 +1761,22 @@
         <v>12</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>88</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E22" s="3">
         <v>2</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>38</v>
@@ -1773,7 +1785,7 @@
         <v>19</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="K22" s="3">
         <v>4.12</v>
@@ -1787,13 +1799,13 @@
         <v>12</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>88</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E23" s="3">
         <v>4</v>
@@ -1802,16 +1814,16 @@
         <v>94</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="K23" s="3">
         <v>1.01</v>
@@ -1825,22 +1837,22 @@
         <v>12</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>88</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E24" s="3">
         <v>6</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>18</v>
@@ -1849,13 +1861,13 @@
         <v>19</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>96</v>
+        <v>124</v>
       </c>
       <c r="K24" s="3">
-        <v>3.2169999999999997E-2</v>
+        <v>0.13411000000000001</v>
       </c>
       <c r="L24" s="3">
-        <v>0.32169999999999999</v>
+        <v>0.80466000000000004</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="15" x14ac:dyDescent="0.4">
@@ -1863,13 +1875,13 @@
         <v>12</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>88</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="E25" s="3">
         <v>2</v>
@@ -1878,7 +1890,7 @@
         <v>94</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>18</v>
@@ -1887,13 +1899,13 @@
         <v>19</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="K25" s="3">
-        <v>0.26806000000000002</v>
+        <v>0.26823000000000002</v>
       </c>
       <c r="L25" s="3">
-        <v>0.53612000000000004</v>
+        <v>0.53646000000000005</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="15" x14ac:dyDescent="0.4">
@@ -1901,13 +1913,13 @@
         <v>12</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>88</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="E26" s="3">
         <v>1</v>
@@ -1916,7 +1928,7 @@
         <v>94</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>18</v>
@@ -1925,13 +1937,13 @@
         <v>19</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="K26" s="3">
-        <v>0.26806000000000002</v>
+        <v>0.26823000000000002</v>
       </c>
       <c r="L26" s="3">
-        <v>0.26806000000000002</v>
+        <v>0.26823000000000002</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="15" x14ac:dyDescent="0.4">
@@ -1939,22 +1951,22 @@
         <v>12</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>88</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="E27" s="3">
         <v>6</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>18</v>
@@ -1963,13 +1975,13 @@
         <v>19</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="K27" s="3">
-        <v>5.8970000000000002E-2</v>
+        <v>5.901E-2</v>
       </c>
       <c r="L27" s="3">
-        <v>0.5897</v>
+        <v>0.59009999999999996</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="15" x14ac:dyDescent="0.4">
@@ -1977,22 +1989,22 @@
         <v>12</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E28" s="3">
         <v>1</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>38</v>
@@ -2001,7 +2013,7 @@
         <v>19</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="K28" s="3">
         <v>0.57669000000000004</v>
@@ -2015,22 +2027,22 @@
         <v>12</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="E29" s="3">
         <v>1</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>18</v>
@@ -2039,13 +2051,13 @@
         <v>19</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="K29" s="3">
-        <v>0.68354000000000004</v>
+        <v>0.68398000000000003</v>
       </c>
       <c r="L29" s="3">
-        <v>0.68354000000000004</v>
+        <v>0.68398000000000003</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="15" x14ac:dyDescent="0.4">
@@ -2053,22 +2065,22 @@
         <v>12</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="E30" s="3">
         <v>1</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>38</v>
@@ -2077,7 +2089,7 @@
         <v>19</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="K30" s="3">
         <v>6.36</v>
@@ -2091,22 +2103,22 @@
         <v>12</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="E31" s="3">
         <v>2</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>38</v>
@@ -2115,7 +2127,7 @@
         <v>19</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="K31" s="3">
         <v>5.82</v>
@@ -2129,22 +2141,22 @@
         <v>12</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="E32" s="3">
         <v>1</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>38</v>
@@ -2153,7 +2165,7 @@
         <v>19</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="K32" s="3">
         <v>0.89856000000000003</v>
@@ -2167,22 +2179,22 @@
         <v>12</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="E33" s="3">
         <v>1</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>38</v>
@@ -2191,7 +2203,7 @@
         <v>19</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="K33" s="3">
         <v>1.82</v>
@@ -2205,22 +2217,22 @@
         <v>12</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="E34" s="3">
         <v>1</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>38</v>
@@ -2229,7 +2241,7 @@
         <v>19</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="K34" s="3">
         <v>0.95220000000000005</v>
@@ -2240,105 +2252,105 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" tooltip="Component" display="'Taiyo Yuden" xr:uid="{18771E8B-FDB4-4FAD-802E-29B49DBD32EE}"/>
-    <hyperlink ref="G2" r:id="rId2" tooltip="Manufacturer" display="'EMK105B7104KVHF" xr:uid="{2EAF0A50-FEF2-41FF-8955-91EC5F8EA2A1}"/>
-    <hyperlink ref="J2" r:id="rId3" tooltip="Supplier" display="'587-3807-1-ND" xr:uid="{3D6D0111-C020-46FE-A800-1A80ABC5E2F6}"/>
-    <hyperlink ref="F3" r:id="rId4" tooltip="Component" display="'Murata" xr:uid="{99A73993-6180-4552-A8CE-341600167838}"/>
-    <hyperlink ref="G3" r:id="rId5" tooltip="Manufacturer" display="'GCM1555C1H150FA16D" xr:uid="{9B15F92E-7ABB-41EC-8505-C94E79AA77CB}"/>
-    <hyperlink ref="J3" r:id="rId6" tooltip="Supplier" display="'490-14350-6-ND" xr:uid="{C0D4550F-CC1F-4622-86DE-E99FF721270F}"/>
-    <hyperlink ref="F4" r:id="rId7" tooltip="Component" display="'United Chemi-Con" xr:uid="{C95878BC-1DC8-4B84-AC9B-F08DCBB09752}"/>
-    <hyperlink ref="G4" r:id="rId8" tooltip="Manufacturer" display="'KTJ500B476M76BFT00" xr:uid="{ED8E14F2-5C9D-4984-BE9B-5BE26FCD8E5D}"/>
-    <hyperlink ref="J4" r:id="rId9" tooltip="Supplier" display="'565-4687-6-ND" xr:uid="{8BE304AF-48F9-4244-A110-63DFFB379D04}"/>
-    <hyperlink ref="F5" r:id="rId10" tooltip="Component" display="'KEMET" xr:uid="{F6C50CD1-8C7F-45BD-AEED-BA6E1BFBF020}"/>
-    <hyperlink ref="G5" r:id="rId11" tooltip="Manufacturer" display="'C0603C104K5RACAUTO" xr:uid="{F81B0A33-3BA0-423A-B14A-4537942AD811}"/>
-    <hyperlink ref="J5" r:id="rId12" tooltip="Supplier" display="'399-6856-6-ND" xr:uid="{D5365D33-5805-491E-AD7F-8FF855D05F47}"/>
-    <hyperlink ref="F6" r:id="rId13" tooltip="Component" display="'Wurth Electronics" xr:uid="{41E6B94A-7A09-437D-91DB-D599F24B5677}"/>
-    <hyperlink ref="G6" r:id="rId14" tooltip="Manufacturer" display="'885012206001" xr:uid="{1DCFC22B-7A4D-4342-8FA6-C2E53F5AE67B}"/>
-    <hyperlink ref="J6" r:id="rId15" tooltip="Supplier" display="'732-7920-6-ND" xr:uid="{594F233F-DAF6-47D0-8EBD-FFC34383EFD0}"/>
-    <hyperlink ref="F7" r:id="rId16" tooltip="Component" display="'KEMET" xr:uid="{E6CA0C9F-BEA1-48E1-8C05-F3578134CD08}"/>
-    <hyperlink ref="G7" r:id="rId17" tooltip="Manufacturer" display="'C0805F103K5RACAUTO" xr:uid="{2D192D76-6AE3-4D2B-BD22-CC492C194B3F}"/>
-    <hyperlink ref="J7" r:id="rId18" tooltip="Supplier" display="'399-6982-6-ND" xr:uid="{8513A89D-237E-4DCB-8A3A-860AF65A024F}"/>
-    <hyperlink ref="F8" r:id="rId19" tooltip="Component" display="'Rohm" xr:uid="{4CAC650F-5366-434F-B390-8AF6AA1263E1}"/>
-    <hyperlink ref="G8" r:id="rId20" tooltip="Manufacturer" display="'SML-D12U1WT86" xr:uid="{66FA4FCF-1E0D-4DFD-9079-C99B4A5E13F1}"/>
-    <hyperlink ref="J8" r:id="rId21" tooltip="Supplier" display="'SML-D12U1WT86DKR-ND" xr:uid="{BE00630D-2F21-44F4-83D3-EC92210CD8B0}"/>
-    <hyperlink ref="F9" r:id="rId22" tooltip="Component" display="'Rohm" xr:uid="{BBC8786A-F18B-46ED-9493-7471826D5B7F}"/>
-    <hyperlink ref="G9" r:id="rId23" tooltip="Manufacturer" display="'SML-D12FWT86" xr:uid="{88E35193-0C90-42F7-A073-B918782DC87F}"/>
-    <hyperlink ref="J9" r:id="rId24" tooltip="Supplier" display="'846-1176-6-ND" xr:uid="{00E616B6-A614-407A-92CF-DC0F011C1B94}"/>
-    <hyperlink ref="F10" r:id="rId25" tooltip="Component" display="'Rohm" xr:uid="{8C901A45-E860-4319-9467-4DDF4B57510C}"/>
-    <hyperlink ref="G10" r:id="rId26" tooltip="Manufacturer" display="'SML-D12D8WT86" xr:uid="{1389DC25-B71B-4B4D-B9B6-14E333DC6726}"/>
-    <hyperlink ref="J10" r:id="rId27" tooltip="Supplier" display="'511-1577-6-ND" xr:uid="{6099B3A2-6E6D-46D3-9FDF-B4B60C211580}"/>
-    <hyperlink ref="F11" tooltip="Component" display="'" xr:uid="{62B1C4E2-A481-47A0-B025-69E1407A65CE}"/>
-    <hyperlink ref="G11" tooltip="Manufacturer" display="'" xr:uid="{E320252B-427F-48BB-9C6A-C51A093BC39D}"/>
-    <hyperlink ref="J11" tooltip="Supplier" display="'" xr:uid="{75426CDB-B892-4E93-8A8A-869A6F747EE5}"/>
-    <hyperlink ref="F12" r:id="rId28" tooltip="Component" display="'Wurth Electronics" xr:uid="{C538B486-058E-4A10-8B3B-5E7E930658EA}"/>
-    <hyperlink ref="G12" r:id="rId29" tooltip="Manufacturer" display="'691102710002" xr:uid="{C6B6DB12-BEDA-4272-89A3-AB00F2D1960C}"/>
-    <hyperlink ref="J12" r:id="rId30" tooltip="Supplier" display="'732-2028-ND" xr:uid="{7526BDD7-88F5-41EB-AB19-2BDD56862786}"/>
-    <hyperlink ref="F13" r:id="rId31" tooltip="Component" display="'Samtec" xr:uid="{E146E344-F98C-41A2-9858-37BEEBF84660}"/>
-    <hyperlink ref="G13" r:id="rId32" tooltip="Manufacturer" display="'SFMC-102-01-S-D" xr:uid="{B79E24AD-9A28-4A93-8A40-31351AA91E74}"/>
-    <hyperlink ref="J13" r:id="rId33" tooltip="Supplier" display="'SAM9900-ND" xr:uid="{1D23EA99-90DB-4014-A5C1-85155D7F695B}"/>
-    <hyperlink ref="F14" r:id="rId34" tooltip="Component" display="'Samtec" xr:uid="{B58F8C1F-2DB1-4770-9079-3E7342FCCD28}"/>
-    <hyperlink ref="G14" r:id="rId35" tooltip="Manufacturer" display="'SLW-103-01-L-D" xr:uid="{F570BEDE-53A5-442D-AB36-AD1AC1CBEE5D}"/>
-    <hyperlink ref="J14" r:id="rId36" tooltip="Supplier" display="'SAM12856-ND" xr:uid="{3762B3ED-00B3-488C-A41B-F1B340E50778}"/>
-    <hyperlink ref="F15" r:id="rId37" tooltip="Component" display="'Hirose" xr:uid="{BF4CB851-D8B6-4FE9-B9A5-B02024331BEE}"/>
-    <hyperlink ref="G15" r:id="rId38" tooltip="Manufacturer" display="'DF13A-4P-1.25H(21)" xr:uid="{3D407BA9-4C0C-41D4-8A31-D2E0C3DF6855}"/>
-    <hyperlink ref="J15" r:id="rId39" tooltip="Supplier" display="'H125082-CT-ND" xr:uid="{A9678579-0D54-4680-B71E-139CE8F2CB52}"/>
-    <hyperlink ref="F16" r:id="rId40" tooltip="Component" display="'Vishay Beyschlag" xr:uid="{283454EF-3234-4E2E-AFEE-004D55B2C792}"/>
-    <hyperlink ref="G16" r:id="rId41" tooltip="Manufacturer" display="'MCT06030C3001FP500" xr:uid="{B2FD740D-370E-47DE-BB8A-F4979D7CC8E8}"/>
-    <hyperlink ref="J16" r:id="rId42" tooltip="Supplier" display="'MCT0603-3.00K-CFCT-ND" xr:uid="{C530214C-7622-4CE7-B1CA-53BB0541C8AC}"/>
-    <hyperlink ref="F17" r:id="rId43" tooltip="Component" display="'Yageo" xr:uid="{D6655B39-1247-41E8-9FB9-9909B6B0A32F}"/>
-    <hyperlink ref="G17" r:id="rId44" tooltip="Manufacturer" display="'RC0603FR-07330RL" xr:uid="{172B9F7C-357B-4B82-9D95-0914CDFB6CCF}"/>
-    <hyperlink ref="J17" r:id="rId45" tooltip="Supplier" display="'311-330HRCT-ND" xr:uid="{221A87E9-DA84-4B98-AC0B-41F9FDE80B55}"/>
-    <hyperlink ref="F18" r:id="rId46" tooltip="Component" display="'Panasonic" xr:uid="{8A1AB03D-D260-4DDA-8F07-EDBB5917E7F8}"/>
-    <hyperlink ref="G18" r:id="rId47" tooltip="Manufacturer" display="'ERA-3AEB303V" xr:uid="{22597244-8771-4DF2-83BE-637F753B0195}"/>
-    <hyperlink ref="J18" r:id="rId48" tooltip="Supplier" display="'P30KDBDKR-ND" xr:uid="{F23F5755-701A-4BBE-B93A-A8DE06692703}"/>
-    <hyperlink ref="F19" r:id="rId49" tooltip="Component" display="'Panasonic" xr:uid="{695A6D5A-94CA-49BD-9F73-5FFCB583B19B}"/>
-    <hyperlink ref="G19" r:id="rId50" tooltip="Manufacturer" display="'ERA-3AEB303V" xr:uid="{921C2B54-5357-4E7A-B9B4-AEFF6FCC2AB9}"/>
-    <hyperlink ref="J19" r:id="rId51" tooltip="Supplier" display="'P30KDBDKR-ND" xr:uid="{28D8498D-D261-4478-A590-A114DAE1652B}"/>
-    <hyperlink ref="F20" r:id="rId52" tooltip="Component" display="'Yageo" xr:uid="{0EE6E5C8-211F-4FA0-9798-D3E70B6B6A7C}"/>
-    <hyperlink ref="G20" r:id="rId53" tooltip="Manufacturer" display="'RT0603DRD0710KL" xr:uid="{56D1C82C-DFEF-4788-BF8E-B0DE8AD59FFA}"/>
-    <hyperlink ref="J20" r:id="rId54" tooltip="Supplier" display="'311-10KDCT-ND" xr:uid="{40FF4990-83EF-4A20-81E8-713C8619262D}"/>
-    <hyperlink ref="F21" r:id="rId55" tooltip="Component" display="'Vishay Beyschlag" xr:uid="{FEAE978B-B2B9-46FC-8E78-745754AF2FA7}"/>
-    <hyperlink ref="G21" r:id="rId56" tooltip="Manufacturer" display="'MCT06030C1004FP500" xr:uid="{C2A83942-BF74-4ED1-AE4E-B30AFFC5315E}"/>
-    <hyperlink ref="J21" r:id="rId57" tooltip="Supplier" display="'MCT0603-1.00M-CFTR-ND" xr:uid="{BB5FECCF-F4AC-4FA1-9D7E-B3FBDD3557E9}"/>
-    <hyperlink ref="F22" r:id="rId58" tooltip="Component" display="'Vishay Dale Thin Film" xr:uid="{DEC4E1D3-7CF5-404F-8AB0-9C501F813A62}"/>
-    <hyperlink ref="G22" r:id="rId59" tooltip="Manufacturer" display="'PNM0603E5002BST5" xr:uid="{B4CB6071-E1B0-4903-8B4C-6DEE30EB6C06}"/>
-    <hyperlink ref="J22" r:id="rId60" tooltip="Supplier" display="'PNM0603-50KBCT-ND" xr:uid="{4046AC04-E00D-4FAF-802D-0295C3BFC26A}"/>
-    <hyperlink ref="F23" r:id="rId61" tooltip="Component" display="'Yageo" xr:uid="{83781FD0-25C0-460F-9591-5FC428D441C8}"/>
-    <hyperlink ref="G23" r:id="rId62" tooltip="Manufacturer" display="'SR0805FR-471RL" xr:uid="{66A78141-E059-458A-9FC9-4593B0F631B8}"/>
-    <hyperlink ref="J23" r:id="rId63" tooltip="Supplier" display="'YAG5851CT-ND" xr:uid="{6ED912A6-B5B7-433F-998B-D49538374549}"/>
-    <hyperlink ref="F24" r:id="rId64" tooltip="Component" display="'Yageo" xr:uid="{F085709E-0192-4BC1-8FDF-A0D1B2124AC7}"/>
-    <hyperlink ref="G24" r:id="rId65" tooltip="Manufacturer" display="'RC0603FR-07330RL" xr:uid="{065DC4D6-3C21-41D1-AC56-1B7B6046D0DE}"/>
-    <hyperlink ref="J24" r:id="rId66" tooltip="Supplier" display="'311-330HRCT-ND" xr:uid="{80BF6FF9-196F-4567-BCB2-B159A9DA3B49}"/>
-    <hyperlink ref="F25" r:id="rId67" tooltip="Component" display="'Yageo" xr:uid="{43254AED-02C0-465F-B68C-532BA944E432}"/>
-    <hyperlink ref="G25" r:id="rId68" tooltip="Manufacturer" display="'RT0603DRD0710KL" xr:uid="{4F47818B-F1E9-4E8C-8AD3-74713161F7EA}"/>
-    <hyperlink ref="J25" r:id="rId69" tooltip="Supplier" display="'311-10KDCT-ND" xr:uid="{5D52EC49-D92D-4741-B958-FF82E04BAEBB}"/>
-    <hyperlink ref="F26" r:id="rId70" tooltip="Component" display="'Yageo" xr:uid="{882AE138-5919-41BA-96BC-66B1D658EB05}"/>
-    <hyperlink ref="G26" r:id="rId71" tooltip="Manufacturer" display="'RT0603DRD0710KL" xr:uid="{DFB2F4F4-FAB2-4D3E-A821-220185728F46}"/>
-    <hyperlink ref="J26" r:id="rId72" tooltip="Supplier" display="'311-10KDCT-ND" xr:uid="{4D5B260B-5784-4A92-8B2A-D16B85F1C5DF}"/>
-    <hyperlink ref="F27" r:id="rId73" tooltip="Component" display="'Vishay" xr:uid="{60E347B5-9218-40EC-9EE8-D5E73FF58F38}"/>
-    <hyperlink ref="G27" r:id="rId74" tooltip="Manufacturer" display="'CRCW08050000Z0EA" xr:uid="{47C0855C-3381-4683-A9A2-7A27033811B2}"/>
-    <hyperlink ref="J27" r:id="rId75" tooltip="Supplier" display="'541-0.0ACT-ND" xr:uid="{CACCB0B6-7957-46BE-81F9-9AEA46751BA1}"/>
-    <hyperlink ref="F28" r:id="rId76" tooltip="Component" display="'ITT C&amp;K" xr:uid="{E2E0FC84-6A9F-425B-90F8-8CB8A766EB8E}"/>
-    <hyperlink ref="G28" r:id="rId77" tooltip="Manufacturer" display="'JS202011AQN" xr:uid="{8835F7A1-0F57-41B1-AEC0-AB600A8BD1EB}"/>
-    <hyperlink ref="J28" r:id="rId78" tooltip="Supplier" display="'401-2000-ND" xr:uid="{DE9B5BA1-7401-4C2E-B7ED-61615BDA3D62}"/>
-    <hyperlink ref="F29" r:id="rId79" tooltip="Component" display="'ITT C&amp;K" xr:uid="{34F2BA0E-92ED-4A58-9C4D-92C38763EFBD}"/>
-    <hyperlink ref="G29" r:id="rId80" tooltip="Manufacturer" display="'PTS830GM140SMTRLFS" xr:uid="{2B3E364A-4C04-4EFE-88C4-E947D8056CF8}"/>
-    <hyperlink ref="J29" r:id="rId81" tooltip="Supplier" display="'CKN10587DKR-ND" xr:uid="{56B9DF67-A9B6-434F-8F30-CD9A132FC4F2}"/>
-    <hyperlink ref="F30" r:id="rId82" tooltip="Component" display="'Microchip / Atmel" xr:uid="{D329788E-D2FF-43DA-8C39-EC992BA50038}"/>
-    <hyperlink ref="G30" r:id="rId83" tooltip="Manufacturer" display="'ATMEGA32M1-AUR" xr:uid="{D8F07582-040D-4836-AA74-A0A6FE54EC44}"/>
-    <hyperlink ref="J30" r:id="rId84" tooltip="Supplier" display="'ATMEGA32M1-AURCT-ND" xr:uid="{71E57E9D-59F7-4596-A7D6-C5ED09F7E5E2}"/>
-    <hyperlink ref="F31" r:id="rId85" tooltip="Component" display="'Texas Instruments" xr:uid="{DC8778C6-FDB5-44F5-B775-2328020B6785}"/>
-    <hyperlink ref="G31" r:id="rId86" tooltip="Manufacturer" display="'DRV8843PWP" xr:uid="{F3F54C5F-C30D-4951-A67F-0195B23C6872}"/>
-    <hyperlink ref="J31" r:id="rId87" tooltip="Supplier" display="'296-28918-5-ND" xr:uid="{AC8CDB94-25E0-4AEE-BD8E-E486EBF53690}"/>
-    <hyperlink ref="F32" r:id="rId88" tooltip="Component" display="'Texas Instruments" xr:uid="{ACAF157A-6C95-4069-99D2-7621C2A0E0DD}"/>
-    <hyperlink ref="G32" r:id="rId89" tooltip="Manufacturer" display="'SN74HC365PW" xr:uid="{382C50E0-EF8F-42E1-99DE-62AAEB06C4EE}"/>
-    <hyperlink ref="J32" r:id="rId90" tooltip="Supplier" display="'296-33932-5-ND" xr:uid="{B2A4580C-3E8A-4C0F-98A5-95B67C223C31}"/>
-    <hyperlink ref="F33" r:id="rId91" tooltip="Component" display="'Microchip" xr:uid="{F3DAB133-090B-41E7-B56D-EA72A0F8C05F}"/>
-    <hyperlink ref="G33" r:id="rId92" tooltip="Manufacturer" display="'MCP23S17-E/SS" xr:uid="{07A50EB2-DF41-4897-B779-381AAB2CEABB}"/>
-    <hyperlink ref="J33" r:id="rId93" tooltip="Supplier" display="'MCP23S17-E/SS-ND" xr:uid="{A38F6AC8-F0A2-4AE5-B97A-0EE4D4C99132}"/>
-    <hyperlink ref="F34" r:id="rId94" tooltip="Component" display="'Abracon" xr:uid="{9B54D63B-5AC7-4880-9728-F2073D7F87B0}"/>
-    <hyperlink ref="G34" r:id="rId95" tooltip="Manufacturer" display="'ABM3B-8.000MHZ-10-D-1-G-T" xr:uid="{21AC7600-BF0B-4224-B81C-F6B0A9BD9EC8}"/>
-    <hyperlink ref="J34" r:id="rId96" tooltip="Supplier" display="'535-13456-1-ND" xr:uid="{D9F533F9-EF81-4104-B493-061952F12F6C}"/>
+    <hyperlink ref="F2" r:id="rId1" tooltip="Component" display="'Taiyo Yuden" xr:uid="{348A82BA-F7C7-4967-BBC1-D6A274AD11E7}"/>
+    <hyperlink ref="G2" r:id="rId2" tooltip="Manufacturer" display="'EMK105B7104KVHF" xr:uid="{E7BE070E-C148-4A49-9ACA-C727A4841C6C}"/>
+    <hyperlink ref="J2" r:id="rId3" tooltip="Supplier" display="'587-3807-1-ND" xr:uid="{8FB9FE0B-663F-42D2-B08A-B38EF19F08F6}"/>
+    <hyperlink ref="F3" r:id="rId4" tooltip="Component" display="'Murata" xr:uid="{4240CB98-4CE8-41DB-A269-7CF43A9310EA}"/>
+    <hyperlink ref="G3" r:id="rId5" tooltip="Manufacturer" display="'GRM1555C1H150FA01D" xr:uid="{2FBBB30A-C913-4929-BDD7-8C31890E1CA4}"/>
+    <hyperlink ref="J3" r:id="rId6" tooltip="Supplier" display="'490-6200-1-ND" xr:uid="{EDC64B07-822E-499D-BF9D-4F371CBED913}"/>
+    <hyperlink ref="F4" r:id="rId7" tooltip="Component" display="'United Chemi-Con" xr:uid="{31761946-EAFA-4BF5-8A56-C739BE064CF6}"/>
+    <hyperlink ref="G4" r:id="rId8" tooltip="Manufacturer" display="'KTJ500B476M76BFT00" xr:uid="{852FF1E6-DDCD-4FE5-9043-E0AA9E5CA5B5}"/>
+    <hyperlink ref="J4" r:id="rId9" tooltip="Supplier" display="'565-4687-1-ND" xr:uid="{804A6E14-6DF5-4EE4-9A16-8893E93BB70C}"/>
+    <hyperlink ref="F5" r:id="rId10" tooltip="Component" display="'KEMET" xr:uid="{CA6AAC3B-ECF5-44A9-88E5-58D37AA1635C}"/>
+    <hyperlink ref="G5" r:id="rId11" tooltip="Manufacturer" display="'C0603C104K5RACAUTO" xr:uid="{32D1B376-3CBC-4F73-82C5-9E0523301DFC}"/>
+    <hyperlink ref="J5" r:id="rId12" tooltip="Supplier" display="'399-6856-1-ND" xr:uid="{CEC4F4C2-374C-4ED9-9337-ADD872BDE392}"/>
+    <hyperlink ref="F6" r:id="rId13" tooltip="Component" display="'Wurth Electronics" xr:uid="{D1FA2D93-FBE6-4C79-8796-721143EA5BDC}"/>
+    <hyperlink ref="G6" r:id="rId14" tooltip="Manufacturer" display="'885012206001" xr:uid="{19931372-45B0-4B4F-97CD-1C843C89A4C2}"/>
+    <hyperlink ref="J6" r:id="rId15" tooltip="Supplier" display="'732-7920-1-ND" xr:uid="{A5639624-3C37-4580-AC3E-F6CC786D2AA5}"/>
+    <hyperlink ref="F7" r:id="rId16" tooltip="Component" display="'KEMET" xr:uid="{18030DC0-3FC9-497D-9AB2-F42E707B641F}"/>
+    <hyperlink ref="G7" r:id="rId17" tooltip="Manufacturer" display="'C0805F103K5RACAUTO" xr:uid="{9D8647C1-7CFF-4DD5-8D2C-546EA7AFD314}"/>
+    <hyperlink ref="J7" r:id="rId18" tooltip="Supplier" display="'399-6982-1-ND" xr:uid="{DCB08E46-0B30-4560-B6AC-61E5B92B2BB7}"/>
+    <hyperlink ref="F8" r:id="rId19" tooltip="Component" display="'Rohm" xr:uid="{39DDD5E8-8E67-4B1C-A9FC-F64A6CA1F1D1}"/>
+    <hyperlink ref="G8" r:id="rId20" tooltip="Manufacturer" display="'SML-D12U1WT86" xr:uid="{2D501CFA-55DC-4284-9293-61888623DDA2}"/>
+    <hyperlink ref="J8" r:id="rId21" tooltip="Supplier" display="'SML-D12U1WT86CT-ND" xr:uid="{B6DE9980-1394-4764-BC07-79C2EE768489}"/>
+    <hyperlink ref="F9" r:id="rId22" tooltip="Component" display="'Rohm" xr:uid="{FA24235B-C4DA-40DC-97C3-F0279CABEAC2}"/>
+    <hyperlink ref="G9" r:id="rId23" tooltip="Manufacturer" display="'SML-D12FWT86" xr:uid="{EF6E45E7-F018-4561-9CDF-A06910A28390}"/>
+    <hyperlink ref="J9" r:id="rId24" tooltip="Supplier" display="'846-1176-1-ND" xr:uid="{1A062474-BB5A-4C35-80B4-056A31498F08}"/>
+    <hyperlink ref="F10" r:id="rId25" tooltip="Component" display="'Rohm" xr:uid="{D8CA5B53-63C2-4FF1-B3A5-46F26C957FFD}"/>
+    <hyperlink ref="G10" r:id="rId26" tooltip="Manufacturer" display="'SML-D12D8WT86" xr:uid="{2285C37F-1FFB-4FA9-93B5-C7286DA4CDF9}"/>
+    <hyperlink ref="J10" r:id="rId27" tooltip="Supplier" display="'511-1577-1-ND" xr:uid="{ABEE8250-3F98-4D0A-916F-BD554780D2E1}"/>
+    <hyperlink ref="F11" tooltip="Component" display="'" xr:uid="{44338C83-8FF9-4AF8-B23F-C3ECABFA4AE9}"/>
+    <hyperlink ref="G11" tooltip="Manufacturer" display="'" xr:uid="{965AD464-C364-44C0-9E50-E00C4706CE2B}"/>
+    <hyperlink ref="J11" tooltip="Supplier" display="'" xr:uid="{69F3C410-7888-4F4B-BD33-32917A93686B}"/>
+    <hyperlink ref="F12" r:id="rId28" tooltip="Component" display="'Wurth Electronics" xr:uid="{C72239AE-DCF4-4072-A4BA-CBFA45BA5C0B}"/>
+    <hyperlink ref="G12" r:id="rId29" tooltip="Manufacturer" display="'691102710002" xr:uid="{9F3C14DC-A9A4-40C5-8334-FB46D35A9F56}"/>
+    <hyperlink ref="J12" r:id="rId30" tooltip="Supplier" display="'732-2028-ND" xr:uid="{55888677-915A-4476-BD2F-7A0580AA68E7}"/>
+    <hyperlink ref="F13" r:id="rId31" tooltip="Component" display="'Samtec" xr:uid="{5143E671-9B76-4CC3-9D32-B5E6DB9CD4AB}"/>
+    <hyperlink ref="G13" r:id="rId32" tooltip="Manufacturer" display="'SFMC-102-01-S-D" xr:uid="{43E0BC37-C605-4EB8-9486-C1CC5463E4FC}"/>
+    <hyperlink ref="J13" r:id="rId33" tooltip="Supplier" display="'SAM9900-ND" xr:uid="{55529F93-264F-4188-9BAE-1FAD9CFC19E1}"/>
+    <hyperlink ref="F14" r:id="rId34" tooltip="Component" display="'Samtec" xr:uid="{346D4100-0104-4344-86D0-4CBB3855A559}"/>
+    <hyperlink ref="G14" r:id="rId35" tooltip="Manufacturer" display="'SLW-103-01-L-D" xr:uid="{6106F0BE-E784-456C-8562-910228251708}"/>
+    <hyperlink ref="J14" r:id="rId36" tooltip="Supplier" display="'SAM12856-ND" xr:uid="{51EA7D17-70D8-4AE6-95DB-9109418EE6D5}"/>
+    <hyperlink ref="F15" r:id="rId37" tooltip="Component" display="'Hirose" xr:uid="{A45C8BE3-DDD0-4260-B44F-22233FB13731}"/>
+    <hyperlink ref="G15" r:id="rId38" tooltip="Manufacturer" display="'DF13A-4P-1.25H(21)" xr:uid="{2DB3B225-75D7-4F34-A1F6-388B5F6CCFA0}"/>
+    <hyperlink ref="J15" r:id="rId39" tooltip="Supplier" display="'H125082-CT-ND" xr:uid="{9CB15446-8DBF-44FA-972B-75694FDE9454}"/>
+    <hyperlink ref="F16" r:id="rId40" tooltip="Component" display="'Vishay Beyschlag" xr:uid="{52BA8F5D-8503-46EC-A47F-442F4F3EBA47}"/>
+    <hyperlink ref="G16" r:id="rId41" tooltip="Manufacturer" display="'MCT06030C3001FP500" xr:uid="{125D3C94-D84B-469B-A9A8-4DC07900F00F}"/>
+    <hyperlink ref="J16" r:id="rId42" tooltip="Supplier" display="'MCT0603-3.00K-CFCT-ND" xr:uid="{0738948E-10DE-4F8F-A3E4-CE6B9EDD7A2F}"/>
+    <hyperlink ref="F17" r:id="rId43" tooltip="Component" display="'Yageo" xr:uid="{7D10FD65-3FB2-4F3B-8868-FBA39CD0C271}"/>
+    <hyperlink ref="G17" r:id="rId44" tooltip="Manufacturer" display="'RC0603FR-07330RL" xr:uid="{235C5AC7-B30C-4249-9049-3D65401BA9B4}"/>
+    <hyperlink ref="J17" r:id="rId45" tooltip="Supplier" display="'311-330HRCT-ND" xr:uid="{96543CDF-51AE-4702-B21E-2E98B43932D4}"/>
+    <hyperlink ref="F18" r:id="rId46" tooltip="Component" display="'Panasonic" xr:uid="{53B28E39-587F-4493-B6E6-55F59508FC3A}"/>
+    <hyperlink ref="G18" r:id="rId47" tooltip="Manufacturer" display="'ERJ-2RKF3002X" xr:uid="{424245C1-3E53-4D70-B526-4F00B89AC03A}"/>
+    <hyperlink ref="J18" r:id="rId48" tooltip="Supplier" display="'P30.0KLCT-ND" xr:uid="{0A4A377A-9E4C-44B6-94AC-595EFEE53763}"/>
+    <hyperlink ref="F19" r:id="rId49" tooltip="Component" display="'Panasonic" xr:uid="{0CEB8D44-89F8-42BE-9830-FB857DEC14C1}"/>
+    <hyperlink ref="G19" r:id="rId50" tooltip="Manufacturer" display="'ERA-3AEB303V" xr:uid="{0FBFE8BF-8800-437B-A6B2-4B7317873FBC}"/>
+    <hyperlink ref="J19" r:id="rId51" tooltip="Supplier" display="'P30KDBCT-ND" xr:uid="{A70F16BE-A0DB-4BBF-8D96-3761A0D9F3FA}"/>
+    <hyperlink ref="F20" r:id="rId52" tooltip="Component" display="'Yageo" xr:uid="{DBABB70F-B822-4975-A07F-6D7D4B26E541}"/>
+    <hyperlink ref="G20" r:id="rId53" tooltip="Manufacturer" display="'RT0603DRD0710KL" xr:uid="{ACAB9F55-9C34-4167-9587-B34805E19678}"/>
+    <hyperlink ref="J20" r:id="rId54" tooltip="Supplier" display="'311-10KDCT-ND" xr:uid="{F3D60876-0BD4-49AF-8D94-F02589F52A46}"/>
+    <hyperlink ref="F21" r:id="rId55" tooltip="Component" display="'Vishay Beyschlag" xr:uid="{EA346A9B-11DD-477B-A02F-61F31A1E4FBD}"/>
+    <hyperlink ref="G21" r:id="rId56" tooltip="Manufacturer" display="'MCT06030C1004FP500" xr:uid="{ECA8F886-217D-4B98-A4E8-D310EF1C6837}"/>
+    <hyperlink ref="J21" r:id="rId57" tooltip="Supplier" display="'MCT0603-1.00M-CFCT-ND" xr:uid="{048A1E27-C6FA-43EC-B926-4A0FC4A483D8}"/>
+    <hyperlink ref="F22" r:id="rId58" tooltip="Component" display="'Vishay Dale Thin Film" xr:uid="{E81C567A-5958-4607-98D4-07FE3C23DDB6}"/>
+    <hyperlink ref="G22" r:id="rId59" tooltip="Manufacturer" display="'PNM0603E5002BST5" xr:uid="{1259770B-394F-4EDC-9FD2-79F3E46D7271}"/>
+    <hyperlink ref="J22" r:id="rId60" tooltip="Supplier" display="'PNM0603-50KBCT-ND" xr:uid="{9E84C84A-2DFA-4012-861B-650945130DDC}"/>
+    <hyperlink ref="F23" r:id="rId61" tooltip="Component" display="'Yageo" xr:uid="{07514985-0B52-4A10-936E-643B3DE81C3A}"/>
+    <hyperlink ref="G23" r:id="rId62" tooltip="Manufacturer" display="'SR0805FR-471RL" xr:uid="{9B098A64-82FB-4CE5-B77D-C30A52BF600A}"/>
+    <hyperlink ref="J23" r:id="rId63" tooltip="Supplier" display="'YAG5851CT-ND" xr:uid="{C0B55180-EA18-4B8B-8352-0A4C3C3C5888}"/>
+    <hyperlink ref="F24" r:id="rId64" tooltip="Component" display="'Panasonic" xr:uid="{25AD00AC-91C3-4989-A6AD-5E24FD42BC24}"/>
+    <hyperlink ref="G24" r:id="rId65" tooltip="Manufacturer" display="'ERJ3EKF3300V" xr:uid="{D192F630-E4B5-49FA-928B-F50159885F2D}"/>
+    <hyperlink ref="J24" r:id="rId66" tooltip="Supplier" display="'P330HCT-ND" xr:uid="{62D2C7E2-06F8-464F-B35E-AF4796E9DC45}"/>
+    <hyperlink ref="F25" r:id="rId67" tooltip="Component" display="'Yageo" xr:uid="{B668A245-6E40-474C-8406-9D63BB1476A5}"/>
+    <hyperlink ref="G25" r:id="rId68" tooltip="Manufacturer" display="'RT0603DRD0710KL" xr:uid="{5A59C537-EBD1-457A-9DAC-F75123A74D75}"/>
+    <hyperlink ref="J25" r:id="rId69" tooltip="Supplier" display="'311-10KDCT-ND" xr:uid="{90E09A4E-2A96-4815-A7B8-F72D77470D81}"/>
+    <hyperlink ref="F26" r:id="rId70" tooltip="Component" display="'Yageo" xr:uid="{9D9970C4-775B-4A51-8EA3-F70E792C23D8}"/>
+    <hyperlink ref="G26" r:id="rId71" tooltip="Manufacturer" display="'RT0603DRD0710KL" xr:uid="{513334CA-DB9A-4E9B-B341-120A8FC4BE1C}"/>
+    <hyperlink ref="J26" r:id="rId72" tooltip="Supplier" display="'311-10KDCT-ND" xr:uid="{D28BFE56-9DC6-4392-8873-34CB41F7620F}"/>
+    <hyperlink ref="F27" r:id="rId73" tooltip="Component" display="'Vishay" xr:uid="{1EE4C09C-4DC9-4EDD-B5D5-F4EA01DA0C3C}"/>
+    <hyperlink ref="G27" r:id="rId74" tooltip="Manufacturer" display="'CRCW08050000Z0EA" xr:uid="{4760A094-3107-4CCE-B568-86F17491A8DA}"/>
+    <hyperlink ref="J27" r:id="rId75" tooltip="Supplier" display="'541-0.0ACT-ND" xr:uid="{3915C6A2-56ED-4517-9943-FEC9F9858299}"/>
+    <hyperlink ref="F28" r:id="rId76" tooltip="Component" display="'ITT C&amp;K" xr:uid="{3EC5E95F-E7AF-4480-AD16-6353C19FC523}"/>
+    <hyperlink ref="G28" r:id="rId77" tooltip="Manufacturer" display="'JS202011AQN" xr:uid="{379E664E-E96D-4BC2-A3B7-863BCD6960CC}"/>
+    <hyperlink ref="J28" r:id="rId78" tooltip="Supplier" display="'401-2000-ND" xr:uid="{D3A5D0E7-053A-45D2-AC2A-93D87B47EBD4}"/>
+    <hyperlink ref="F29" r:id="rId79" tooltip="Component" display="'ITT C&amp;K" xr:uid="{199119C3-1AEC-4149-95CF-E0355185324E}"/>
+    <hyperlink ref="G29" r:id="rId80" tooltip="Manufacturer" display="'PTS830GM140SMTRLFS" xr:uid="{AF0AF8AD-24BE-4ADA-B448-30406D357186}"/>
+    <hyperlink ref="J29" r:id="rId81" tooltip="Supplier" display="'CKN10587CT-ND" xr:uid="{693F7B46-62D1-4D2E-AF56-14F58BB6D44F}"/>
+    <hyperlink ref="F30" r:id="rId82" tooltip="Component" display="'Microchip / Atmel" xr:uid="{7515766B-BF8F-440C-A982-46BCB841FAF0}"/>
+    <hyperlink ref="G30" r:id="rId83" tooltip="Manufacturer" display="'ATMEGA32M1-AUR" xr:uid="{AD558356-1B6B-4E27-A23E-D8C55E98F7E3}"/>
+    <hyperlink ref="J30" r:id="rId84" tooltip="Supplier" display="'ATMEGA32M1-AURCT-ND" xr:uid="{7422AFA9-3227-46AC-A9AD-F21A4234966B}"/>
+    <hyperlink ref="F31" r:id="rId85" tooltip="Component" display="'Texas Instruments" xr:uid="{60344643-6E4E-465F-9ADA-AEE599F2513F}"/>
+    <hyperlink ref="G31" r:id="rId86" tooltip="Manufacturer" display="'DRV8843PWP" xr:uid="{F6677ECD-92C8-4F70-AC32-A046CF531E77}"/>
+    <hyperlink ref="J31" r:id="rId87" tooltip="Supplier" display="'296-28918-5-ND" xr:uid="{693D4D25-F0D7-46B6-9C2E-45BCD3A910ED}"/>
+    <hyperlink ref="F32" r:id="rId88" tooltip="Component" display="'Texas Instruments" xr:uid="{8AB7608B-52C9-4C7B-A62B-2648E39BF474}"/>
+    <hyperlink ref="G32" r:id="rId89" tooltip="Manufacturer" display="'SN74HC365PW" xr:uid="{7CB1B348-BE64-40EC-946A-0765A0AE271A}"/>
+    <hyperlink ref="J32" r:id="rId90" tooltip="Supplier" display="'296-33932-5-ND" xr:uid="{C7D464A4-05DE-4C17-A1A3-6089A76E3D0A}"/>
+    <hyperlink ref="F33" r:id="rId91" tooltip="Component" display="'Microchip" xr:uid="{90169CA4-4912-483B-9F6E-D0C47C1FB12D}"/>
+    <hyperlink ref="G33" r:id="rId92" tooltip="Manufacturer" display="'MCP23S17-E/SS" xr:uid="{78EA10AB-C8DF-4052-B121-4D14C064D833}"/>
+    <hyperlink ref="J33" r:id="rId93" tooltip="Supplier" display="'MCP23S17-E/SS-ND" xr:uid="{607A8347-D785-4598-98FE-B13F3FE063E4}"/>
+    <hyperlink ref="F34" r:id="rId94" tooltip="Component" display="'Abracon" xr:uid="{648527AD-0408-49AA-8FAF-EA505E9F658B}"/>
+    <hyperlink ref="G34" r:id="rId95" tooltip="Manufacturer" display="'ABM3B-8.000MHZ-10-D-1-G-T" xr:uid="{6974B215-02DD-425A-B357-5BED23074069}"/>
+    <hyperlink ref="J34" r:id="rId96" tooltip="Supplier" display="'535-13456-1-ND" xr:uid="{3BA20568-5C64-4658-A52D-4AE777DDF408}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId97"/>

</xml_diff>